<commit_message>
adding age categories that comply with LOB divisions and with business at DHCS/actuary
</commit_message>
<xml_diff>
--- a/Docs/Project/Project-Artifacts/Reference-Material/LIBRARY/__HospitalReadmissionLiteratureReview_LindaJones.xlsx
+++ b/Docs/Project/Project-Artifacts/Reference-Material/LIBRARY/__HospitalReadmissionLiteratureReview_LindaJones.xlsx
@@ -128,9 +128,6 @@
     <t>Graham, K. L., Dike, O., Doctoroff, L., Jupiter, M., Vanka, A., Davis, R. B., &amp; Marcantonio, E. R. (2017). Preventability of early vs. late readmissions in an academic medical center. PLoS ONE, 12(6), e0178718. http://doi.org/10.1371/journal.pone.0178718</t>
   </si>
   <si>
-    <t xml:space="preserve">Readmissions were significantly more preventable in the early compared to the late period. Patients readmitted in the early period were significantly more likely to have mental status changes documented 24h prior to hospital discharge than patients readmitted in the late period </t>
-  </si>
-  <si>
     <t>Compare preventability of hospital readmissions, between an early period [0–7 days post-discharge] and a late period [8–30 days post-discharge]. Compare causes of readmission, and frequency of markers of clinical instability 24h prior to discharge between early and late readmissions.</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>developed an algorithm for identifying inpatients at high risk of re-admission to a National Health Service (NHS) hospital in England within 30 days of discharge using information that can either be obtained from hospital information systems or from the patient and their notes.</t>
   </si>
   <si>
-    <t>We have developed a method of identifying inpatients at high risk of unplanned re-admission to NHS hospitals within 30 days of discharge. Though the models had a low sensitivity, we show how to identify subgroups of patients that contain a high proportion of patients who will be re-admitted within 30 days. Additional work is necessary to validate the model in practice</t>
-  </si>
-  <si>
     <t>Billings, J., Blunt, I., Steventon, A., Georghiou, T., Lewis, G., &amp; Bardsley, M. (2012). Development of a predictive model to identify inpatients at risk of re-admission within 30 days of discharge (PARR-30). BMJ Open, 2(4), e001667. http://doi.org/10.1136/bmjopen-2012-001667</t>
   </si>
   <si>
@@ -231,13 +225,50 @@
   </si>
   <si>
     <t xml:space="preserve">Clinical Research Databases, randomly split study population </t>
+  </si>
+  <si>
+    <r>
+      <t>Readmissions were significantly more preventable in the early compared to the late period.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Patients readmitted in the early period were significantly more likely to have mental status changes documented 24h prior to hospital discharge than patients readmitted in the late period </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We have developed a method of identifying inpatients at high risk of unplanned re-admission to NHS hospitals within 30 days of discharge. Though the models had a low sensitivity, we show how to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>identify subgroups of patients</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that contain a high proportion of patients who will be re-admitted within 30 days. Additional work is necessary to validate the model in practice</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,8 +295,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -452,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -490,7 +533,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -779,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
@@ -789,7 +841,7 @@
     <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="86.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="125.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="79.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="154.5703125" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
@@ -840,7 +892,7 @@
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="4"/>
@@ -873,7 +925,7 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -882,7 +934,7 @@
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H4" s="4"/>
@@ -913,128 +965,128 @@
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="16" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="101.25" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="121.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="81" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="G10" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="203.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="G11" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="H11" s="4"/>
     </row>

</xml_diff>